<commit_message>
Add additional fields for verification for node properties parity
</commit_message>
<xml_diff>
--- a/InputFiles/API/MDB/CypherQueries.xlsx
+++ b/InputFiles/API/MDB/CypherQueries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/API/MDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC501554-65CA-6147-B77A-E5CCD2D6C4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBB0460-4858-0E4A-A456-BDD5F4E64A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="-22380" windowWidth="39620" windowHeight="17800" xr2:uid="{E31DFAE0-8367-D64E-B72E-FBCDBE56359A}"/>
+    <workbookView xWindow="12500" yWindow="-23600" windowWidth="39620" windowHeight="17800" xr2:uid="{E31DFAE0-8367-D64E-B72E-FBCDBE56359A}"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>key</t>
   </si>
@@ -93,6 +93,14 @@
 m.nanoid AS nanoid, 
 m.is_latest_version AS is_latest_version 
 ORDER BY handle, version</t>
+  </si>
+  <si>
+    <t>MATCH (n:node { model: $modelHandle, version: $versionString, handle: $nodeHandle })
+			MATCH (n)-[:has_property]-&gt;(p:property)
+			RETURN p</t>
+  </si>
+  <si>
+    <t>verifyModelNodePropertiesEmpty</t>
   </si>
 </sst>
 </file>
@@ -485,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8CE0E7-003B-DB4B-B327-82B56A12C61B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,6 +545,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add MDB property terms verification
</commit_message>
<xml_diff>
--- a/InputFiles/API/MDB/CypherQueries.xlsx
+++ b/InputFiles/API/MDB/CypherQueries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/API/MDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBB0460-4858-0E4A-A456-BDD5F4E64A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3FF49-3D02-F642-8397-7FA1B2FC4524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12500" yWindow="-23600" windowWidth="39620" windowHeight="17800" xr2:uid="{E31DFAE0-8367-D64E-B72E-FBCDBE56359A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>key</t>
   </si>
@@ -101,6 +101,38 @@
   </si>
   <si>
     <t>verifyModelNodePropertiesEmpty</t>
+  </si>
+  <si>
+    <t>verifyModelNodePropertyTerms</t>
+  </si>
+  <si>
+    <t>MATCH (n:node { model: $modelHandle, version: $versionString, handle: $nodeHandle })
+MATCH (n)-[:has_property]-&gt;(p:property { handle: $propHandle })
+MATCH (p)-[:has_value_set]-&gt;(vs:value_set)
+MATCH (vs)-[:has_term]-&gt;(t:term)
+RETURN
+  n.model          AS model,
+  n.version        AS version,
+  n.handle         AS node,
+  p.handle         AS property,
+  t.value          AS value,
+  t.handle         AS handle,
+  t.origin_name    AS origin_name,
+  t.origin_version AS origin_version,
+  t.origin_id      AS origin_id,
+  t.nanoid         AS nanoid
+ORDER BY value, nanoid</t>
+  </si>
+  <si>
+    <t>verifyModelNodePropertyTermsEmpty</t>
+  </si>
+  <si>
+    <t>MATCH (n:node { model: $modelHandle, version: $versionString, handle: $nodeHandle })
+MATCH (n)-[:has_property]-&gt;(p:property { handle: $propHandle })
+MATCH (p)-[:has_value_set]-&gt;(vs:value_set)
+MATCH (vs)-[:has_term]-&gt;(t:term)
+RETURN t.nanoid AS nanoid
+LIMIT 1</t>
   </si>
 </sst>
 </file>
@@ -493,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8CE0E7-003B-DB4B-B327-82B56A12C61B}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,6 +585,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:2" ht="272" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>